<commit_message>
programação das figuras do grupo 15, antes feitas por Rodrigo
</commit_message>
<xml_diff>
--- a/Data/g15.1.xlsx
+++ b/Data/g15.1.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -392,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>7.8</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7.7</v>
       </c>
     </row>
     <row r="3">
@@ -412,11 +488,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>8.199999999999999</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7.8</v>
       </c>
     </row>
     <row r="4">
@@ -432,11 +508,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>9.199999999999999</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8.1</v>
       </c>
     </row>
     <row r="5">
@@ -452,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>9.199999999999999</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9.5</v>
       </c>
     </row>
     <row r="6">
@@ -472,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>9.300000000000001</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>8.4</v>
       </c>
     </row>
     <row r="7">
@@ -492,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>8.9</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9.4</v>
       </c>
     </row>
     <row r="8">
@@ -512,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>8.800000000000001</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +608,10 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D9">
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>7.6</v>
       </c>
     </row>
@@ -552,11 +628,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>6.3</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>7.1</v>
       </c>
     </row>
     <row r="11">
@@ -572,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>5.9</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>6.3</v>
       </c>
     </row>
     <row r="12">
@@ -592,11 +668,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>5.4</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>5.1</v>
       </c>
     </row>
     <row r="13">
@@ -612,11 +688,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>3.6</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.3</v>
       </c>
     </row>
     <row r="14">
@@ -632,11 +708,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>3.3</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -652,11 +728,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>2.4</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2.6</v>
       </c>
     </row>
     <row r="16">
@@ -672,10 +748,10 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D16">
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -692,10 +768,10 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D17">
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>1.1</v>
       </c>
     </row>
@@ -712,11 +788,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>31/12/2014</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>1.3</v>
+          <t>01/01/2015</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="19">
@@ -732,10 +808,10 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D19">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>7.5</v>
       </c>
     </row>
@@ -752,10 +828,10 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D20">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>7.7</v>
       </c>
     </row>
@@ -772,10 +848,10 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D21">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>8</v>
       </c>
     </row>
@@ -792,10 +868,10 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D22">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>9</v>
       </c>
     </row>
@@ -812,10 +888,10 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D23">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>9</v>
       </c>
     </row>
@@ -832,10 +908,10 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D24">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>8.699999999999999</v>
       </c>
     </row>
@@ -852,10 +928,10 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D25">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>8</v>
       </c>
     </row>
@@ -872,10 +948,10 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D26">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>8.199999999999999</v>
       </c>
     </row>
@@ -892,10 +968,10 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D27">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>7.5</v>
       </c>
     </row>
@@ -912,10 +988,10 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D28">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>6.1</v>
       </c>
     </row>
@@ -932,10 +1008,10 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D29">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>5.3</v>
       </c>
     </row>
@@ -952,10 +1028,10 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D30">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>4</v>
       </c>
     </row>
@@ -972,10 +1048,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D31">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>3.3</v>
       </c>
     </row>
@@ -992,10 +1068,10 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D32">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>2.6</v>
       </c>
     </row>
@@ -1012,10 +1088,10 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D33">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>1.9</v>
       </c>
     </row>
@@ -1032,10 +1108,10 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D34">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -1052,10 +1128,10 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D35">
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1072,10 +1148,10 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D36">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
         <v>7.5</v>
       </c>
     </row>
@@ -1092,10 +1168,10 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D37">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
         <v>8.1</v>
       </c>
     </row>
@@ -1112,10 +1188,10 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D38">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
         <v>7.1</v>
       </c>
     </row>
@@ -1132,10 +1208,10 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D39">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
         <v>7.8</v>
       </c>
     </row>
@@ -1152,10 +1228,10 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D40">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>8.4</v>
       </c>
     </row>
@@ -1172,10 +1248,10 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D41">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
         <v>7.9</v>
       </c>
     </row>
@@ -1192,10 +1268,10 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D42">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
         <v>8.199999999999999</v>
       </c>
     </row>
@@ -1212,10 +1288,10 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D43">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
         <v>7.4</v>
       </c>
     </row>
@@ -1232,10 +1308,10 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D44">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
         <v>7.3</v>
       </c>
     </row>
@@ -1252,10 +1328,10 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D45">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>6.8</v>
       </c>
     </row>
@@ -1272,10 +1348,10 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D46">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
         <v>5.4</v>
       </c>
     </row>
@@ -1292,10 +1368,10 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D47">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
         <v>5.3</v>
       </c>
     </row>
@@ -1312,10 +1388,10 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D48">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -1332,10 +1408,10 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D49">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
         <v>2.9</v>
       </c>
     </row>
@@ -1352,10 +1428,10 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D50">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1372,10 +1448,10 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D51">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1392,14 +1468,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>31/12/2023</t>
-        </is>
-      </c>
-      <c r="D52">
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
         <v>2.1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>